<commit_message>
Version 2.3 mit 64 Bit-Positionswerten ohne serielle Kommunikation zum Achsmodul
</commit_message>
<xml_diff>
--- a/src/sample/src/ssc_project/CiA402Example.xlsx
+++ b/src/sample/src/ssc_project/CiA402Example.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b20467ae3810cfc8/Studium/Semester/6. Semester/Fachpraktikum/EtherCAT_CiA402/1_Workspace/workspace_selfmade_ssc/1_V2.2/EtherCAT_SSC_CiA402/src/sample/src/ssc_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b20467ae3810cfc8/Studium/Semester/6. Semester/Fachpraktikum/EtherCAT_CiA402/1_Workspace/workspace_selfmade_ssc/1_V2.x/EtherCAT_SSC_CiA402/src/sample/src/ssc_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_BDFEFDA0D73BD2C085FB18E7AF2BC5402792095B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A0833D4-ABA1-41F9-9AD3-B0539014C8CF}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_BDFEFDA0D73BD2C085FB18E7AF2BC5402792095B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1632459-524F-48E6-BA5E-4B0DD5F459F3}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27516" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Profile" sheetId="11" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Profile!$B$10:$P$118</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Profile!$B$1:$P$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Profile!$B$10:$P$120</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Profile!$B$1:$P$121</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="168">
   <si>
     <t>Index</t>
   </si>
@@ -641,6 +641,15 @@
   </si>
   <si>
     <t>Axis 0 objects (0x6000 - 0x67FF)</t>
+  </si>
+  <si>
+    <t>INT64</t>
+  </si>
+  <si>
+    <t>0x607A0040</t>
+  </si>
+  <si>
+    <t>0x60640040</t>
   </si>
 </sst>
 </file>
@@ -1111,11 +1120,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T969"/>
+  <dimension ref="A1:T971"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
+      <pane ySplit="10" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1124,7 +1133,7 @@
     <col min="2" max="2" width="20.33203125" style="16" customWidth="1"/>
     <col min="3" max="5" width="14.6640625" style="16" customWidth="1"/>
     <col min="6" max="6" width="40.6640625" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="7.6640625" style="16" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="16" customWidth="1"/>
     <col min="11" max="11" width="7.6640625" style="16" customWidth="1"/>
@@ -1836,7 +1845,7 @@
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="13" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -2356,7 +2365,7 @@
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="13" t="s">
-        <v>124</v>
+        <v>167</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
@@ -2484,7 +2493,7 @@
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
@@ -2497,7 +2506,7 @@
       <c r="N56"/>
       <c r="O56"/>
       <c r="P56" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:16" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -3363,13 +3372,13 @@
       <c r="C94" s="4"/>
       <c r="D94" s="11"/>
       <c r="E94" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="F94" t="s">
         <v>83</v>
       </c>
-      <c r="G94" t="s">
-        <v>151</v>
+      <c r="G94">
+        <v>0</v>
       </c>
       <c r="H94" s="22"/>
       <c r="I94" s="22"/>
@@ -3509,13 +3518,13 @@
       <c r="C100" s="4"/>
       <c r="D100" s="11"/>
       <c r="E100" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="F100" t="s">
         <v>91</v>
       </c>
-      <c r="G100" t="s">
-        <v>151</v>
+      <c r="G100">
+        <v>0</v>
       </c>
       <c r="H100" s="22"/>
       <c r="I100" s="22"/>
@@ -3953,106 +3962,84 @@
       <c r="O118"/>
       <c r="P118"/>
     </row>
-    <row r="119" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="13"/>
-      <c r="B119" s="14" t="s">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A119" s="4"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="4"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="4"/>
+      <c r="L119" s="4"/>
+      <c r="M119" s="4"/>
+      <c r="N119"/>
+      <c r="O119"/>
+      <c r="P119"/>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A120" s="4"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="4"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="4"/>
+      <c r="L120" s="4"/>
+      <c r="M120" s="4"/>
+      <c r="N120"/>
+      <c r="O120"/>
+      <c r="P120"/>
+    </row>
+    <row r="121" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="13"/>
+      <c r="B121" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="C119" s="14" t="s">
+      <c r="C121" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14"/>
-      <c r="G119" s="14"/>
-      <c r="H119" s="14"/>
-      <c r="I119" s="14"/>
-      <c r="J119" s="14"/>
-      <c r="K119" s="14"/>
-      <c r="L119" s="14"/>
-      <c r="M119" s="14"/>
-      <c r="N119" s="14"/>
-      <c r="O119" s="14"/>
-      <c r="P119" s="14"/>
-    </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="14"/>
+      <c r="G121" s="14"/>
+      <c r="H121" s="14"/>
+      <c r="I121" s="14"/>
+      <c r="J121" s="14"/>
+      <c r="K121" s="14"/>
+      <c r="L121" s="14"/>
+      <c r="M121" s="14"/>
+      <c r="N121" s="14"/>
+      <c r="O121" s="14"/>
+      <c r="P121" s="14"/>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
         <v>40</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C122" t="s">
         <v>95</v>
       </c>
-      <c r="D120"/>
-      <c r="E120"/>
-      <c r="F120" t="s">
+      <c r="D122"/>
+      <c r="E122"/>
+      <c r="F122" t="s">
         <v>136</v>
       </c>
-      <c r="G120"/>
-      <c r="H120"/>
-      <c r="I120"/>
-      <c r="J120" t="s">
-        <v>70</v>
-      </c>
-      <c r="K120"/>
-      <c r="L120"/>
-      <c r="M120"/>
-      <c r="N120"/>
-      <c r="O120" s="4"/>
-      <c r="P120" s="4"/>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B121"/>
-      <c r="C121"/>
-      <c r="D121">
-        <v>1</v>
-      </c>
-      <c r="E121" t="s">
-        <v>66</v>
-      </c>
-      <c r="F121" t="s">
-        <v>137</v>
-      </c>
-      <c r="G121" t="s">
-        <v>141</v>
-      </c>
-      <c r="H121"/>
-      <c r="I121"/>
-      <c r="J121" t="s">
-        <v>70</v>
-      </c>
-      <c r="K121"/>
-      <c r="L121" t="s">
-        <v>77</v>
-      </c>
-      <c r="M121"/>
-      <c r="N121" s="23"/>
-      <c r="O121" s="4"/>
-      <c r="P121" s="4"/>
-    </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B122"/>
-      <c r="C122"/>
-      <c r="D122">
-        <v>2</v>
-      </c>
-      <c r="E122" t="s">
-        <v>66</v>
-      </c>
-      <c r="F122" t="s">
-        <v>138</v>
-      </c>
-      <c r="G122" t="s">
-        <v>156</v>
-      </c>
+      <c r="G122"/>
       <c r="H122"/>
       <c r="I122"/>
       <c r="J122" t="s">
         <v>70</v>
       </c>
       <c r="K122"/>
-      <c r="L122" t="s">
-        <v>77</v>
-      </c>
+      <c r="L122"/>
       <c r="M122"/>
       <c r="N122"/>
       <c r="O122" s="4"/>
@@ -4061,35 +4048,51 @@
     <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B123"/>
       <c r="C123"/>
-      <c r="D123"/>
-      <c r="E123"/>
-      <c r="F123"/>
-      <c r="G123"/>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" t="s">
+        <v>66</v>
+      </c>
+      <c r="F123" t="s">
+        <v>137</v>
+      </c>
+      <c r="G123" t="s">
+        <v>141</v>
+      </c>
       <c r="H123"/>
       <c r="I123"/>
-      <c r="J123"/>
+      <c r="J123" t="s">
+        <v>70</v>
+      </c>
       <c r="K123"/>
-      <c r="L123"/>
+      <c r="L123" t="s">
+        <v>77</v>
+      </c>
       <c r="M123"/>
-      <c r="N123"/>
+      <c r="N123" s="23"/>
+      <c r="O123" s="4"/>
+      <c r="P123" s="4"/>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
-        <v>41</v>
-      </c>
-      <c r="C124" t="s">
-        <v>139</v>
-      </c>
-      <c r="D124"/>
-      <c r="E124"/>
+      <c r="B124"/>
+      <c r="C124"/>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124" t="s">
+        <v>66</v>
+      </c>
       <c r="F124" t="s">
-        <v>140</v>
-      </c>
-      <c r="G124"/>
+        <v>138</v>
+      </c>
+      <c r="G124" t="s">
+        <v>156</v>
+      </c>
       <c r="H124"/>
       <c r="I124"/>
       <c r="J124" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K124"/>
       <c r="L124" t="s">
@@ -4097,59 +4100,71 @@
       </c>
       <c r="M124"/>
       <c r="N124"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="4"/>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B125"/>
       <c r="C125"/>
-      <c r="D125">
-        <v>1</v>
-      </c>
-      <c r="E125" t="s">
-        <v>93</v>
-      </c>
+      <c r="D125"/>
+      <c r="E125"/>
       <c r="F125"/>
-      <c r="G125" t="s">
-        <v>142</v>
-      </c>
+      <c r="G125"/>
       <c r="H125"/>
       <c r="I125"/>
-      <c r="J125" t="s">
-        <v>68</v>
-      </c>
+      <c r="J125"/>
       <c r="K125"/>
-      <c r="L125" t="s">
-        <v>77</v>
-      </c>
+      <c r="L125"/>
       <c r="M125"/>
       <c r="N125"/>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B126"/>
-      <c r="C126"/>
+      <c r="B126" t="s">
+        <v>41</v>
+      </c>
+      <c r="C126" t="s">
+        <v>139</v>
+      </c>
       <c r="D126"/>
       <c r="E126"/>
-      <c r="F126"/>
+      <c r="F126" t="s">
+        <v>140</v>
+      </c>
       <c r="G126"/>
       <c r="H126"/>
       <c r="I126"/>
-      <c r="J126"/>
+      <c r="J126" t="s">
+        <v>68</v>
+      </c>
       <c r="K126"/>
-      <c r="L126"/>
+      <c r="L126" t="s">
+        <v>77</v>
+      </c>
       <c r="M126"/>
       <c r="N126"/>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B127"/>
       <c r="C127"/>
-      <c r="D127"/>
-      <c r="E127"/>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127" t="s">
+        <v>93</v>
+      </c>
       <c r="F127"/>
-      <c r="G127"/>
+      <c r="G127" t="s">
+        <v>142</v>
+      </c>
       <c r="H127"/>
       <c r="I127"/>
-      <c r="J127"/>
+      <c r="J127" t="s">
+        <v>68</v>
+      </c>
       <c r="K127"/>
-      <c r="L127"/>
+      <c r="L127" t="s">
+        <v>77</v>
+      </c>
       <c r="M127"/>
       <c r="N127"/>
     </row>
@@ -4259,10 +4274,34 @@
       <c r="N134"/>
     </row>
     <row r="135" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C135" s="4"/>
+      <c r="B135"/>
+      <c r="C135"/>
+      <c r="D135"/>
+      <c r="E135"/>
+      <c r="F135"/>
+      <c r="G135"/>
+      <c r="H135"/>
+      <c r="I135"/>
+      <c r="J135"/>
+      <c r="K135"/>
+      <c r="L135"/>
+      <c r="M135"/>
+      <c r="N135"/>
     </row>
     <row r="136" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C136" s="4"/>
+      <c r="B136"/>
+      <c r="C136"/>
+      <c r="D136"/>
+      <c r="E136"/>
+      <c r="F136"/>
+      <c r="G136"/>
+      <c r="H136"/>
+      <c r="I136"/>
+      <c r="J136"/>
+      <c r="K136"/>
+      <c r="L136"/>
+      <c r="M136"/>
+      <c r="N136"/>
     </row>
     <row r="137" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C137" s="4"/>
@@ -6762,6 +6801,12 @@
     </row>
     <row r="969" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C969" s="4"/>
+    </row>
+    <row r="970" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C970" s="4"/>
+    </row>
+    <row r="971" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C971" s="4"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatRows="0" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0"/>
@@ -6770,20 +6815,20 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:M13 M15:M16 M18:M19 M39:M40 M42:M59 M61:M63 M65:M74 M76:M118 M21:M37" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:M13 M15:M16 M18:M19 M39:M40 M42:M59 M61:M63 M65:M74 M76:M120 M21:M37" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"rx,tx"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C42:C59 C61:C63 C65:C74 C39:C40 C76:C118 C21:C37" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Object Code value" error="The Object code value shall be:_x000a_VARIABLE_x000a_RECORD_x000a_ARRAY" sqref="C12:C13 C15:C16 C18:C19 C42:C59 C61:C63 C65:C74 C39:C40 C76:C120 C21:C37" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C38 C41 C60 C64 C75 C119 D120:D134" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J42:J59 J61:J63 J65:J74 J39:J40 J76:J118 J21:J37" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="C11 C14 C17 C20 C38 C41 C60 C64 C75 C121 D122:D136" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Category" error="The value for the entry category shall be _x000a_M : (mandatory)_x000a_O : (optional) _x000a_C : (conditional)" sqref="J12:J13 J15:J16 J18:J19 J42:J59 J61:J63 J65:J74 J39:J40 J76:J120 J21:J37" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"M,O,C"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K42:K59 K61:K63 K65:K74 K39:K40 K76:K118 K21:K37" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Backup/Setting Flag" error="The entry flag shall be_x000a_B : (Backup)_x000a_S : (Setting)" sqref="K12:K13 K15:K16 K18:K19 K42:K59 K61:K63 K65:K74 K39:K40 K76:K120 K21:K37" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"B,S"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C135:C969" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C137:C971" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"VARIABLE,ARRAY,RECORD"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>